<commit_message>
Massive code clean up and update some tests
Signed-off-by: Chin Yeung Li <tli@nexb.com>
</commit_message>
<xml_diff>
--- a/samples/report_sample.xlsx
+++ b/samples/report_sample.xlsx
@@ -13,9 +13,9 @@
     <sheet name="D2D" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOM!$A$1:$AV$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOM!$A$1:$AV$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">D2D!$C$1:$H$98</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">BOM!$A$1:$S$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">BOM!$A$1:$S$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">README!$A$1:$B$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">BOM!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">D2D!$1:$1</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="103">
   <si>
     <t>Description</t>
   </si>
@@ -216,34 +216,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>CommScope</t>
-  </si>
-  <si>
-    <t>LKM</t>
-  </si>
-  <si>
-    <t>Dual BSD-GPL</t>
-  </si>
-  <si>
-    <t>dual-bsd-gpl</t>
-  </si>
-  <si>
-    <t>reg</t>
-  </si>
-  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>block</t>
-  </si>
-  <si>
-    <t>kbox.patch</t>
-  </si>
-  <si>
-    <t>pinmux.patch</t>
-  </si>
-  <si>
-    <t>mdio.patch</t>
   </si>
   <si>
     <t>bgrep</t>
@@ -326,39 +299,9 @@
     <t>BSD-Original</t>
   </si>
   <si>
-    <t>jsmn</t>
-  </si>
-  <si>
-    <t>MIT License</t>
-  </si>
-  <si>
-    <t>mit</t>
-  </si>
-  <si>
-    <t>Serge Zaitsev</t>
-  </si>
-  <si>
-    <t>Copyright (c) 2010 Serge A. Zaitsev</t>
-  </si>
-  <si>
-    <t>https://github.com/zserge/jsmn</t>
-  </si>
-  <si>
-    <t>MODP_B64</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
-    <t>http://code.google.com/p/stringencoders/</t>
-  </si>
-  <si>
-    <t>Copyright (c) 2005, 2006, 2007  Nick Galbreath</t>
-  </si>
-  <si>
-    <t>Nick Galbreath</t>
-  </si>
-  <si>
     <t>ninja</t>
   </si>
   <si>
@@ -393,9 +336,6 @@
   </si>
   <si>
     <t>Copyright 2008, Google Inc</t>
-  </si>
-  <si>
-    <t>stringencoders</t>
   </si>
   <si>
     <t>C</t>
@@ -1032,10 +972,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="33" customFormat="1" ht="12" x14ac:dyDescent="0.25">
@@ -1056,7 +996,7 @@
     </row>
     <row r="6" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>0</v>
@@ -1079,12 +1019,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AV14"/>
+  <dimension ref="A1:AV7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1286,19 +1226,19 @@
       <c r="B2" s="14"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F2" s="13">
         <v>3</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>56</v>
@@ -1319,10 +1259,10 @@
         <v>58</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="U2" s="13"/>
       <c r="V2" s="12"/>
@@ -1330,7 +1270,7 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
@@ -1346,7 +1286,7 @@
       <c r="AL2" s="12"/>
       <c r="AM2" s="12"/>
       <c r="AN2" s="12" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="AO2" s="12"/>
       <c r="AP2" s="12"/>
@@ -1362,17 +1302,17 @@
       <c r="B3" s="14"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13">
         <v>3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>56</v>
@@ -1386,7 +1326,7 @@
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="13" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="O3" s="13"/>
       <c r="P3" s="13" t="s">
@@ -1397,7 +1337,7 @@
         <v>58</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
@@ -1406,7 +1346,7 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="AA3" s="12"/>
       <c r="AB3" s="12"/>
@@ -1422,7 +1362,7 @@
       <c r="AL3" s="12"/>
       <c r="AM3" s="12"/>
       <c r="AN3" s="12" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
@@ -1438,22 +1378,22 @@
       <c r="B4" s="14"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F4" s="13">
         <v>3</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>57</v>
@@ -1471,10 +1411,10 @@
         <v>58</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="U4" s="13"/>
       <c r="V4" s="12"/>
@@ -1482,7 +1422,7 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
@@ -1491,7 +1431,7 @@
       <c r="AE4" s="12"/>
       <c r="AF4" s="12"/>
       <c r="AG4" s="12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AH4" s="12"/>
       <c r="AI4" s="12"/>
@@ -1500,7 +1440,7 @@
       <c r="AL4" s="12"/>
       <c r="AM4" s="12"/>
       <c r="AN4" s="12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="AO4" s="12"/>
       <c r="AP4" s="12"/>
@@ -1516,10 +1456,10 @@
       <c r="B5" s="14"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
@@ -1534,7 +1474,7 @@
         <v>56</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13">
@@ -1553,10 +1493,10 @@
         <v>58</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="U5" s="13"/>
       <c r="V5" s="12"/>
@@ -1564,7 +1504,7 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
@@ -1573,7 +1513,7 @@
       <c r="AE5" s="12"/>
       <c r="AF5" s="12"/>
       <c r="AG5" s="12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
@@ -1582,7 +1522,7 @@
       <c r="AL5" s="12"/>
       <c r="AM5" s="12"/>
       <c r="AN5" s="12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
@@ -1594,52 +1534,58 @@
       <c r="AV5" s="12"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="F6" s="13">
         <v>3</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="O6" s="13"/>
       <c r="P6" s="13" t="s">
         <v>58</v>
       </c>
       <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
+      <c r="R6" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="S6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T6" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="U6" s="13"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
+      <c r="Z6" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
@@ -1654,7 +1600,7 @@
       <c r="AL6" s="12"/>
       <c r="AM6" s="12"/>
       <c r="AN6" s="12" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="AO6" s="12"/>
       <c r="AP6" s="12"/>
@@ -1666,24 +1612,26 @@
       <c r="AV6" s="12"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="F7" s="13">
         <v>3</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>57</v>
@@ -1694,9 +1642,7 @@
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="O7" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="O7" s="13"/>
       <c r="P7" s="13" t="s">
         <v>58</v>
       </c>
@@ -1705,15 +1651,19 @@
         <v>58</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T7" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="U7" s="13"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="Z7" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
@@ -1728,7 +1678,7 @@
       <c r="AL7" s="12"/>
       <c r="AM7" s="12"/>
       <c r="AN7" s="12" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="AO7" s="12"/>
       <c r="AP7" s="12"/>
@@ -1738,534 +1688,6 @@
       <c r="AT7" s="12"/>
       <c r="AU7" s="12"/>
       <c r="AV7" s="12"/>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13">
-        <v>3</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13">
-        <v>2</v>
-      </c>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T8" s="12"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="12"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="12"/>
-      <c r="AJ8" s="12"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="12"/>
-      <c r="AM8" s="12"/>
-      <c r="AN8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="12"/>
-      <c r="AQ8" s="12"/>
-      <c r="AR8" s="12"/>
-      <c r="AS8" s="12"/>
-      <c r="AT8" s="12"/>
-      <c r="AU8" s="12"/>
-      <c r="AV8" s="12"/>
-    </row>
-    <row r="9" spans="1:48" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13">
-        <v>2</v>
-      </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" s="12"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="12"/>
-      <c r="AC9" s="12"/>
-      <c r="AD9" s="12"/>
-      <c r="AE9" s="12"/>
-      <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
-      <c r="AH9" s="12"/>
-      <c r="AI9" s="12"/>
-      <c r="AJ9" s="12"/>
-      <c r="AK9" s="12"/>
-      <c r="AL9" s="12"/>
-      <c r="AM9" s="12"/>
-      <c r="AN9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO9" s="12"/>
-      <c r="AP9" s="12"/>
-      <c r="AQ9" s="12"/>
-      <c r="AR9" s="12"/>
-      <c r="AS9" s="12"/>
-      <c r="AT9" s="12"/>
-      <c r="AU9" s="12"/>
-      <c r="AV9" s="12"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13">
-        <v>2</v>
-      </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T10" s="12"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="12"/>
-      <c r="AC10" s="12"/>
-      <c r="AD10" s="12"/>
-      <c r="AE10" s="12"/>
-      <c r="AF10" s="12"/>
-      <c r="AG10" s="12"/>
-      <c r="AH10" s="12"/>
-      <c r="AI10" s="12"/>
-      <c r="AJ10" s="12"/>
-      <c r="AK10" s="12"/>
-      <c r="AL10" s="12"/>
-      <c r="AM10" s="12"/>
-      <c r="AN10" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO10" s="12"/>
-      <c r="AP10" s="12"/>
-      <c r="AQ10" s="12"/>
-      <c r="AR10" s="12"/>
-      <c r="AS10" s="12"/>
-      <c r="AT10" s="12"/>
-      <c r="AU10" s="12"/>
-      <c r="AV10" s="12"/>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13">
-        <v>3</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13">
-        <v>3</v>
-      </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S11" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="12"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
-      <c r="AE11" s="12"/>
-      <c r="AF11" s="12"/>
-      <c r="AG11" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH11" s="12"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="12"/>
-      <c r="AK11" s="12"/>
-      <c r="AL11" s="12"/>
-      <c r="AM11" s="12"/>
-      <c r="AN11" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO11" s="12"/>
-      <c r="AP11" s="12"/>
-      <c r="AQ11" s="12"/>
-      <c r="AR11" s="12"/>
-      <c r="AS11" s="12"/>
-      <c r="AT11" s="12"/>
-      <c r="AU11" s="12"/>
-      <c r="AV11" s="12"/>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13">
-        <v>2</v>
-      </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="U12" s="13"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="12"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="12"/>
-      <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="12"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="12"/>
-      <c r="AM12" s="12"/>
-      <c r="AN12" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="AO12" s="12"/>
-      <c r="AP12" s="12"/>
-      <c r="AQ12" s="12"/>
-      <c r="AR12" s="12"/>
-      <c r="AS12" s="12"/>
-      <c r="AT12" s="12"/>
-      <c r="AU12" s="12"/>
-      <c r="AV12" s="12"/>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13">
-        <v>6</v>
-      </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="U13" s="13"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
-      <c r="AQ13" s="12"/>
-      <c r="AR13" s="12"/>
-      <c r="AS13" s="12"/>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12"/>
-      <c r="AV13" s="12"/>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="13">
-        <v>3</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13">
-        <v>2</v>
-      </c>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="T14" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="U14" s="13"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="12"/>
-      <c r="AJ14" s="12"/>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
-      <c r="AN14" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AO14" s="12"/>
-      <c r="AP14" s="12"/>
-      <c r="AQ14" s="12"/>
-      <c r="AR14" s="12"/>
-      <c r="AS14" s="12"/>
-      <c r="AT14" s="12"/>
-      <c r="AU14" s="12"/>
-      <c r="AV14" s="12"/>
     </row>
   </sheetData>
   <sortState ref="A2:AV25">
@@ -2342,7 +1764,7 @@
     <col min="52" max="52" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="11" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" s="11" customFormat="1" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>